<commit_message>
Update README.md model package add Address.java util package add ExcelFileHandler.java make open api swagger
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -44,16 +44,19 @@
     <t>HR, India</t>
   </si>
   <si>
-    <t>aks</t>
-  </si>
-  <si>
-    <t>aks@gmail.com</t>
-  </si>
-  <si>
-    <t>+911334567891</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> India</t>
+    <t>sdd</t>
+  </si>
+  <si>
+    <t>sdd@gmail.com</t>
+  </si>
+  <si>
+    <t>+911234567891</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>GGN , HR, India</t>
   </si>
   <si>
     <t>erd</t>
@@ -71,19 +74,271 @@
     <t>erd@gmail.com</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>sdd</t>
-  </si>
-  <si>
-    <t>sdd@gmail.com</t>
-  </si>
-  <si>
-    <t>+911234567891</t>
-  </si>
-  <si>
-    <t>GGN , HR, India</t>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>johndoe@example.com</t>
+  </si>
+  <si>
+    <t>+911234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> USA</t>
+  </si>
+  <si>
+    <t>johndoe@gmail.com</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>j@gmail.com</t>
+  </si>
+  <si>
+    <t>+912334567890</t>
+  </si>
+  <si>
+    <t>Jk</t>
+  </si>
+  <si>
+    <t>jk@gmail.com</t>
+  </si>
+  <si>
+    <t>+913334567890</t>
+  </si>
+  <si>
+    <t>azxds</t>
+  </si>
+  <si>
+    <t>zxds@gmail.com</t>
+  </si>
+  <si>
+    <t>+913324567890</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>g@gmail.com</t>
+  </si>
+  <si>
+    <t>+913324567000</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>adsdsd</t>
+  </si>
+  <si>
+    <t>addsd@gmail.com</t>
+  </si>
+  <si>
+    <t>+91004567000</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>erf</t>
+  </si>
+  <si>
+    <t>erfd@gmail.com</t>
+  </si>
+  <si>
+    <t>+91000067000</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>Azad Shukla</t>
+  </si>
+  <si>
+    <t>AzyShukla@gmail.com</t>
+  </si>
+  <si>
+    <t>+911234560091</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>defji@example.com</t>
+  </si>
+  <si>
+    <t>+910034567890</t>
+  </si>
+  <si>
+    <t>134, gen, city,USA</t>
+  </si>
+  <si>
+    <t>sukiji</t>
+  </si>
+  <si>
+    <t>skiji@gmail.com</t>
+  </si>
+  <si>
+    <t>+9800004567890</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Azad</t>
+  </si>
+  <si>
+    <t>Azad@gmail.com</t>
+  </si>
+  <si>
+    <t>+959753231461</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ewwd</t>
+  </si>
+  <si>
+    <t>Azwwd@gmail.com</t>
+  </si>
+  <si>
+    <t>+952353231461</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>gg@gmail.com</t>
+  </si>
+  <si>
+    <t>+942053231423</t>
+  </si>
+  <si>
+    <t>cht</t>
+  </si>
+  <si>
+    <t>ww</t>
+  </si>
+  <si>
+    <t>w.w@gmail.com</t>
+  </si>
+  <si>
+    <t>+191230987654</t>
+  </si>
+  <si>
+    <t>adsa</t>
+  </si>
+  <si>
+    <t>qeccvd</t>
+  </si>
+  <si>
+    <t>dwddwd@gmail.com</t>
+  </si>
+  <si>
+    <t>Henry Ford</t>
+  </si>
+  <si>
+    <t>henry.ford@example.com</t>
+  </si>
+  <si>
+    <t>+331234567891</t>
+  </si>
+  <si>
+    <t>808</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Île-de-France</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>GGN</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Isaac Newton</t>
+  </si>
+  <si>
+    <t>isaac.newton@example.com</t>
+  </si>
+  <si>
+    <t>+611234567890</t>
+  </si>
+  <si>
+    <t>909</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>bob.smith@example.com</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>+112345678913</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>AzadShukla@gmail.com</t>
+  </si>
+  <si>
+    <t>+11234567890</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
   </si>
 </sst>
 </file>
@@ -128,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -153,87 +408,132 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>9</v>
+        <v>93</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>86</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>17</v>
+        <v>86</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>23</v>
+        <v>82</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update README.md update User.java update Address.java update ExcelFileHandler.java update pom.xml update UserRepository.java update UserService.java update userdata.xlsx update UserController.java update data.sql
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -339,6 +339,192 @@
   </si>
   <si>
     <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>hey</t>
+  </si>
+  <si>
+    <t>hey@example.com</t>
+  </si>
+  <si>
+    <t>+96234567890</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>hi@gmail.com</t>
+  </si>
+  <si>
+    <t>+69234567890</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Gg</t>
+  </si>
+  <si>
+    <t>dgg</t>
+  </si>
+  <si>
+    <t>dgg@gmail.com</t>
+  </si>
+  <si>
+    <t>+942400567890</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>asds</t>
+  </si>
+  <si>
+    <t>asad@gmail.com</t>
+  </si>
+  <si>
+    <t>+922400567890</t>
+  </si>
+  <si>
+    <t>Sue</t>
+  </si>
+  <si>
+    <t>sue@gmail.com</t>
+  </si>
+  <si>
+    <t>+18234567890</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>money@gmail.com</t>
+  </si>
+  <si>
+    <t>+25234567890</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>goan</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Ing</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>my@gmail.com</t>
+  </si>
+  <si>
+    <t>+97237777890</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>ghn</t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>jpg@gmail.com</t>
+  </si>
+  <si>
+    <t>+989711794128</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>me@gmail.com</t>
+  </si>
+  <si>
+    <t>+948447120009</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>nmhy</t>
+  </si>
+  <si>
+    <t>nmhy@gmail.com</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>jk</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>shu</t>
+  </si>
+  <si>
+    <t>shu@gmail.com</t>
+  </si>
+  <si>
+    <t>jai</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>heyman</t>
+  </si>
+  <si>
+    <t>heyman@gmail.com</t>
+  </si>
+  <si>
+    <t>+77254567890</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>doller</t>
+  </si>
+  <si>
+    <t>doller@gmail.com</t>
+  </si>
+  <si>
+    <t>+88233367890</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>united</t>
   </si>
 </sst>
 </file>
@@ -383,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -536,6 +722,106 @@
         <v>85</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E10" s="0"/>
+      <c r="F10" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
"Updated User API project: refactored code, added new dependencies, modified configuration files, and updated Excel file handling."
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="207">
   <si>
     <t>Name</t>
   </si>
@@ -525,6 +525,114 @@
   </si>
   <si>
     <t>united</t>
+  </si>
+  <si>
+    <t>+11234567894</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>+859310197424</t>
+  </si>
+  <si>
+    <t>theazadshukla@gmail.com</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>kj</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>+781234567898</t>
+  </si>
+  <si>
+    <t>adi@gmail.com</t>
+  </si>
+  <si>
+    <t>2345</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>dellhi</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>+9998765432167</t>
+  </si>
+  <si>
+    <t>man@gmail.com</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>vice</t>
+  </si>
+  <si>
+    <t>las angle</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>+9912345678956</t>
+  </si>
+  <si>
+    <t>bob@gmail.com</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael </t>
+  </si>
+  <si>
+    <t>+9912345678934</t>
+  </si>
+  <si>
+    <t>Michael@gmail.com</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>Los Santos</t>
+  </si>
+  <si>
+    <t>Los Angle</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>+912345678976</t>
+  </si>
+  <si>
+    <t>jack@gmail.com</t>
+  </si>
+  <si>
+    <t>ggn</t>
+  </si>
+  <si>
+    <t>hr</t>
   </si>
 </sst>
 </file>
@@ -569,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -593,233 +701,351 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="G2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="H2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="I2" t="s" s="0">
         <v>96</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="F3" t="s" s="0">
         <v>86</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>99</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>99</v>
       </c>
       <c r="H3" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s" s="0">
         <v>100</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="F4" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="D7" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>65.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>182</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>66.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>67.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>68.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>69.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="F13" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>105</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>79</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>161</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>163</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>144</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>138</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>158</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" t="s" s="0">
-        <v>159</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>160</v>
-      </c>
-      <c r="H9" t="s" s="0">
+      <c r="G13" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="I13" t="s" s="0">
         <v>35</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>165</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>166</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>167</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E10" s="0"/>
-      <c r="F10" t="s" s="0">
-        <v>168</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>169</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>